<commit_message>
ultimos cambios en reporte y simulacion
</commit_message>
<xml_diff>
--- a/Reportes.xlsx
+++ b/Reportes.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:O261"/>
+  <dimension ref="A1:O301"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -12906,6 +12906,1966 @@
         <v>512</v>
       </c>
     </row>
+    <row r="262">
+      <c r="A262" t="inlineStr">
+        <is>
+          <t>2023-08-21 23:34:18</t>
+        </is>
+      </c>
+      <c r="B262" t="n">
+        <v>40</v>
+      </c>
+      <c r="C262" t="n">
+        <v>13</v>
+      </c>
+      <c r="D262" t="n">
+        <v>8</v>
+      </c>
+      <c r="E262" t="n">
+        <v>2</v>
+      </c>
+      <c r="F262" t="n">
+        <v>7</v>
+      </c>
+      <c r="G262" t="n">
+        <v>4</v>
+      </c>
+      <c r="H262" t="n">
+        <v>26</v>
+      </c>
+      <c r="I262" t="n">
+        <v>16</v>
+      </c>
+      <c r="J262" t="n">
+        <v>17</v>
+      </c>
+      <c r="K262" t="n">
+        <v>0.001</v>
+      </c>
+      <c r="L262" t="n">
+        <v>0.05</v>
+      </c>
+      <c r="M262" t="n">
+        <v>0.003</v>
+      </c>
+      <c r="N262" t="n">
+        <v>70</v>
+      </c>
+      <c r="O262" t="n">
+        <v>512</v>
+      </c>
+    </row>
+    <row r="263">
+      <c r="A263" t="inlineStr">
+        <is>
+          <t>2023-08-21 23:34:23</t>
+        </is>
+      </c>
+      <c r="B263" t="n">
+        <v>40</v>
+      </c>
+      <c r="C263" t="n">
+        <v>19</v>
+      </c>
+      <c r="D263" t="n">
+        <v>7</v>
+      </c>
+      <c r="E263" t="n">
+        <v>1</v>
+      </c>
+      <c r="F263" t="n">
+        <v>11</v>
+      </c>
+      <c r="G263" t="n">
+        <v>7</v>
+      </c>
+      <c r="H263" t="n">
+        <v>45</v>
+      </c>
+      <c r="I263" t="n">
+        <v>12</v>
+      </c>
+      <c r="J263" t="n">
+        <v>17</v>
+      </c>
+      <c r="K263" t="n">
+        <v>0.001</v>
+      </c>
+      <c r="L263" t="n">
+        <v>0.05</v>
+      </c>
+      <c r="M263" t="n">
+        <v>0.003</v>
+      </c>
+      <c r="N263" t="n">
+        <v>70</v>
+      </c>
+      <c r="O263" t="n">
+        <v>512</v>
+      </c>
+    </row>
+    <row r="264">
+      <c r="A264" t="inlineStr">
+        <is>
+          <t>2023-08-21 23:34:35</t>
+        </is>
+      </c>
+      <c r="B264" t="n">
+        <v>130</v>
+      </c>
+      <c r="C264" t="n">
+        <v>62</v>
+      </c>
+      <c r="D264" t="n">
+        <v>7</v>
+      </c>
+      <c r="E264" t="n">
+        <v>11</v>
+      </c>
+      <c r="F264" t="n">
+        <v>27</v>
+      </c>
+      <c r="G264" t="n">
+        <v>24</v>
+      </c>
+      <c r="H264" t="n">
+        <v>39</v>
+      </c>
+      <c r="I264" t="n">
+        <v>25</v>
+      </c>
+      <c r="J264" t="n">
+        <v>18</v>
+      </c>
+      <c r="K264" t="n">
+        <v>0.001</v>
+      </c>
+      <c r="L264" t="n">
+        <v>0.05</v>
+      </c>
+      <c r="M264" t="n">
+        <v>0.003</v>
+      </c>
+      <c r="N264" t="n">
+        <v>70</v>
+      </c>
+      <c r="O264" t="n">
+        <v>512</v>
+      </c>
+    </row>
+    <row r="265">
+      <c r="A265" t="inlineStr">
+        <is>
+          <t>2023-08-21 23:34:47</t>
+        </is>
+      </c>
+      <c r="B265" t="n">
+        <v>120</v>
+      </c>
+      <c r="C265" t="n">
+        <v>64</v>
+      </c>
+      <c r="D265" t="n">
+        <v>6</v>
+      </c>
+      <c r="E265" t="n">
+        <v>10</v>
+      </c>
+      <c r="F265" t="n">
+        <v>23</v>
+      </c>
+      <c r="G265" t="n">
+        <v>31</v>
+      </c>
+      <c r="H265" t="n">
+        <v>31</v>
+      </c>
+      <c r="I265" t="n">
+        <v>28</v>
+      </c>
+      <c r="J265" t="n">
+        <v>9</v>
+      </c>
+      <c r="K265" t="n">
+        <v>0.001</v>
+      </c>
+      <c r="L265" t="n">
+        <v>0.05</v>
+      </c>
+      <c r="M265" t="n">
+        <v>0.003</v>
+      </c>
+      <c r="N265" t="n">
+        <v>70</v>
+      </c>
+      <c r="O265" t="n">
+        <v>512</v>
+      </c>
+    </row>
+    <row r="266">
+      <c r="A266" t="inlineStr">
+        <is>
+          <t>2023-08-21 23:34:59</t>
+        </is>
+      </c>
+      <c r="B266" t="n">
+        <v>118</v>
+      </c>
+      <c r="C266" t="n">
+        <v>56</v>
+      </c>
+      <c r="D266" t="n">
+        <v>9</v>
+      </c>
+      <c r="E266" t="n">
+        <v>18</v>
+      </c>
+      <c r="F266" t="n">
+        <v>21</v>
+      </c>
+      <c r="G266" t="n">
+        <v>17</v>
+      </c>
+      <c r="H266" t="n">
+        <v>25</v>
+      </c>
+      <c r="I266" t="n">
+        <v>19</v>
+      </c>
+      <c r="J266" t="n">
+        <v>23</v>
+      </c>
+      <c r="K266" t="n">
+        <v>0.001</v>
+      </c>
+      <c r="L266" t="n">
+        <v>0.05</v>
+      </c>
+      <c r="M266" t="n">
+        <v>0.003</v>
+      </c>
+      <c r="N266" t="n">
+        <v>70</v>
+      </c>
+      <c r="O266" t="n">
+        <v>512</v>
+      </c>
+    </row>
+    <row r="267">
+      <c r="A267" t="inlineStr">
+        <is>
+          <t>2023-08-22 00:05:04</t>
+        </is>
+      </c>
+      <c r="B267" t="n">
+        <v>40</v>
+      </c>
+      <c r="C267" t="n">
+        <v>14</v>
+      </c>
+      <c r="D267" t="n">
+        <v>7</v>
+      </c>
+      <c r="E267" t="n">
+        <v>3</v>
+      </c>
+      <c r="F267" t="n">
+        <v>5</v>
+      </c>
+      <c r="G267" t="n">
+        <v>6</v>
+      </c>
+      <c r="H267" t="n">
+        <v>23</v>
+      </c>
+      <c r="I267" t="n">
+        <v>33</v>
+      </c>
+      <c r="J267" t="n">
+        <v>10</v>
+      </c>
+      <c r="K267" t="n">
+        <v>0.001</v>
+      </c>
+      <c r="L267" t="n">
+        <v>0.05</v>
+      </c>
+      <c r="M267" t="n">
+        <v>0.003</v>
+      </c>
+      <c r="N267" t="n">
+        <v>75</v>
+      </c>
+      <c r="O267" t="n">
+        <v>512</v>
+      </c>
+    </row>
+    <row r="268">
+      <c r="A268" t="inlineStr">
+        <is>
+          <t>2023-08-22 00:05:13</t>
+        </is>
+      </c>
+      <c r="B268" t="n">
+        <v>40</v>
+      </c>
+      <c r="C268" t="n">
+        <v>22</v>
+      </c>
+      <c r="D268" t="n">
+        <v>12</v>
+      </c>
+      <c r="E268" t="n">
+        <v>2</v>
+      </c>
+      <c r="F268" t="n">
+        <v>11</v>
+      </c>
+      <c r="G268" t="n">
+        <v>9</v>
+      </c>
+      <c r="H268" t="n">
+        <v>43</v>
+      </c>
+      <c r="I268" t="n">
+        <v>12</v>
+      </c>
+      <c r="J268" t="n">
+        <v>17</v>
+      </c>
+      <c r="K268" t="n">
+        <v>0.001</v>
+      </c>
+      <c r="L268" t="n">
+        <v>0.05</v>
+      </c>
+      <c r="M268" t="n">
+        <v>0.003</v>
+      </c>
+      <c r="N268" t="n">
+        <v>75</v>
+      </c>
+      <c r="O268" t="n">
+        <v>512</v>
+      </c>
+    </row>
+    <row r="269">
+      <c r="A269" t="inlineStr">
+        <is>
+          <t>2023-08-22 00:05:36</t>
+        </is>
+      </c>
+      <c r="B269" t="n">
+        <v>130</v>
+      </c>
+      <c r="C269" t="n">
+        <v>53</v>
+      </c>
+      <c r="D269" t="n">
+        <v>9</v>
+      </c>
+      <c r="E269" t="n">
+        <v>8</v>
+      </c>
+      <c r="F269" t="n">
+        <v>28</v>
+      </c>
+      <c r="G269" t="n">
+        <v>17</v>
+      </c>
+      <c r="H269" t="n">
+        <v>63</v>
+      </c>
+      <c r="I269" t="n">
+        <v>12</v>
+      </c>
+      <c r="J269" t="n">
+        <v>24</v>
+      </c>
+      <c r="K269" t="n">
+        <v>0.001</v>
+      </c>
+      <c r="L269" t="n">
+        <v>0.05</v>
+      </c>
+      <c r="M269" t="n">
+        <v>0.003</v>
+      </c>
+      <c r="N269" t="n">
+        <v>75</v>
+      </c>
+      <c r="O269" t="n">
+        <v>512</v>
+      </c>
+    </row>
+    <row r="270">
+      <c r="A270" t="inlineStr">
+        <is>
+          <t>2023-08-22 00:05:59</t>
+        </is>
+      </c>
+      <c r="B270" t="n">
+        <v>120</v>
+      </c>
+      <c r="C270" t="n">
+        <v>55</v>
+      </c>
+      <c r="D270" t="n">
+        <v>7</v>
+      </c>
+      <c r="E270" t="n">
+        <v>11</v>
+      </c>
+      <c r="F270" t="n">
+        <v>22</v>
+      </c>
+      <c r="G270" t="n">
+        <v>22</v>
+      </c>
+      <c r="H270" t="n">
+        <v>66</v>
+      </c>
+      <c r="I270" t="n">
+        <v>13</v>
+      </c>
+      <c r="J270" t="n">
+        <v>22</v>
+      </c>
+      <c r="K270" t="n">
+        <v>0.001</v>
+      </c>
+      <c r="L270" t="n">
+        <v>0.05</v>
+      </c>
+      <c r="M270" t="n">
+        <v>0.003</v>
+      </c>
+      <c r="N270" t="n">
+        <v>75</v>
+      </c>
+      <c r="O270" t="n">
+        <v>512</v>
+      </c>
+    </row>
+    <row r="271">
+      <c r="A271" t="inlineStr">
+        <is>
+          <t>2023-08-22 00:06:21</t>
+        </is>
+      </c>
+      <c r="B271" t="n">
+        <v>118</v>
+      </c>
+      <c r="C271" t="n">
+        <v>49</v>
+      </c>
+      <c r="D271" t="n">
+        <v>16</v>
+      </c>
+      <c r="E271" t="n">
+        <v>13</v>
+      </c>
+      <c r="F271" t="n">
+        <v>25</v>
+      </c>
+      <c r="G271" t="n">
+        <v>11</v>
+      </c>
+      <c r="H271" t="n">
+        <v>30</v>
+      </c>
+      <c r="I271" t="n">
+        <v>19</v>
+      </c>
+      <c r="J271" t="n">
+        <v>32</v>
+      </c>
+      <c r="K271" t="n">
+        <v>0.001</v>
+      </c>
+      <c r="L271" t="n">
+        <v>0.05</v>
+      </c>
+      <c r="M271" t="n">
+        <v>0.003</v>
+      </c>
+      <c r="N271" t="n">
+        <v>75</v>
+      </c>
+      <c r="O271" t="n">
+        <v>512</v>
+      </c>
+    </row>
+    <row r="272">
+      <c r="A272" t="inlineStr">
+        <is>
+          <t>2023-08-22 00:10:21</t>
+        </is>
+      </c>
+      <c r="B272" t="n">
+        <v>40</v>
+      </c>
+      <c r="C272" t="n">
+        <v>20</v>
+      </c>
+      <c r="D272" t="n">
+        <v>4</v>
+      </c>
+      <c r="E272" t="n">
+        <v>5</v>
+      </c>
+      <c r="F272" t="n">
+        <v>5</v>
+      </c>
+      <c r="G272" t="n">
+        <v>10</v>
+      </c>
+      <c r="H272" t="n">
+        <v>14</v>
+      </c>
+      <c r="I272" t="n">
+        <v>18</v>
+      </c>
+      <c r="J272" t="n">
+        <v>10</v>
+      </c>
+      <c r="K272" t="n">
+        <v>0.001</v>
+      </c>
+      <c r="L272" t="n">
+        <v>0.05</v>
+      </c>
+      <c r="M272" t="n">
+        <v>0.003</v>
+      </c>
+      <c r="N272" t="n">
+        <v>70</v>
+      </c>
+      <c r="O272" t="n">
+        <v>512</v>
+      </c>
+    </row>
+    <row r="273">
+      <c r="A273" t="inlineStr">
+        <is>
+          <t>2023-08-22 00:10:30</t>
+        </is>
+      </c>
+      <c r="B273" t="n">
+        <v>40</v>
+      </c>
+      <c r="C273" t="n">
+        <v>24</v>
+      </c>
+      <c r="D273" t="n">
+        <v>6</v>
+      </c>
+      <c r="E273" t="n">
+        <v>6</v>
+      </c>
+      <c r="F273" t="n">
+        <v>9</v>
+      </c>
+      <c r="G273" t="n">
+        <v>9</v>
+      </c>
+      <c r="H273" t="n">
+        <v>12</v>
+      </c>
+      <c r="I273" t="n">
+        <v>11</v>
+      </c>
+      <c r="J273" t="n">
+        <v>14</v>
+      </c>
+      <c r="K273" t="n">
+        <v>0.001</v>
+      </c>
+      <c r="L273" t="n">
+        <v>0.05</v>
+      </c>
+      <c r="M273" t="n">
+        <v>0.003</v>
+      </c>
+      <c r="N273" t="n">
+        <v>70</v>
+      </c>
+      <c r="O273" t="n">
+        <v>512</v>
+      </c>
+    </row>
+    <row r="274">
+      <c r="A274" t="inlineStr">
+        <is>
+          <t>2023-08-22 00:10:55</t>
+        </is>
+      </c>
+      <c r="B274" t="n">
+        <v>130</v>
+      </c>
+      <c r="C274" t="n">
+        <v>54</v>
+      </c>
+      <c r="D274" t="n">
+        <v>18</v>
+      </c>
+      <c r="E274" t="n">
+        <v>5</v>
+      </c>
+      <c r="F274" t="n">
+        <v>29</v>
+      </c>
+      <c r="G274" t="n">
+        <v>20</v>
+      </c>
+      <c r="H274" t="n">
+        <v>46</v>
+      </c>
+      <c r="I274" t="n">
+        <v>22</v>
+      </c>
+      <c r="J274" t="n">
+        <v>18</v>
+      </c>
+      <c r="K274" t="n">
+        <v>0.001</v>
+      </c>
+      <c r="L274" t="n">
+        <v>0.05</v>
+      </c>
+      <c r="M274" t="n">
+        <v>0.003</v>
+      </c>
+      <c r="N274" t="n">
+        <v>70</v>
+      </c>
+      <c r="O274" t="n">
+        <v>512</v>
+      </c>
+    </row>
+    <row r="275">
+      <c r="A275" t="inlineStr">
+        <is>
+          <t>2023-08-22 00:11:18</t>
+        </is>
+      </c>
+      <c r="B275" t="n">
+        <v>120</v>
+      </c>
+      <c r="C275" t="n">
+        <v>57</v>
+      </c>
+      <c r="D275" t="n">
+        <v>7</v>
+      </c>
+      <c r="E275" t="n">
+        <v>9</v>
+      </c>
+      <c r="F275" t="n">
+        <v>23</v>
+      </c>
+      <c r="G275" t="n">
+        <v>25</v>
+      </c>
+      <c r="H275" t="n">
+        <v>25</v>
+      </c>
+      <c r="I275" t="n">
+        <v>15</v>
+      </c>
+      <c r="J275" t="n">
+        <v>10</v>
+      </c>
+      <c r="K275" t="n">
+        <v>0.001</v>
+      </c>
+      <c r="L275" t="n">
+        <v>0.05</v>
+      </c>
+      <c r="M275" t="n">
+        <v>0.003</v>
+      </c>
+      <c r="N275" t="n">
+        <v>70</v>
+      </c>
+      <c r="O275" t="n">
+        <v>512</v>
+      </c>
+    </row>
+    <row r="276">
+      <c r="A276" t="inlineStr">
+        <is>
+          <t>2023-08-22 00:11:40</t>
+        </is>
+      </c>
+      <c r="B276" t="n">
+        <v>118</v>
+      </c>
+      <c r="C276" t="n">
+        <v>49</v>
+      </c>
+      <c r="D276" t="n">
+        <v>8</v>
+      </c>
+      <c r="E276" t="n">
+        <v>9</v>
+      </c>
+      <c r="F276" t="n">
+        <v>19</v>
+      </c>
+      <c r="G276" t="n">
+        <v>21</v>
+      </c>
+      <c r="H276" t="n">
+        <v>32</v>
+      </c>
+      <c r="I276" t="n">
+        <v>15</v>
+      </c>
+      <c r="J276" t="n">
+        <v>16</v>
+      </c>
+      <c r="K276" t="n">
+        <v>0.001</v>
+      </c>
+      <c r="L276" t="n">
+        <v>0.05</v>
+      </c>
+      <c r="M276" t="n">
+        <v>0.003</v>
+      </c>
+      <c r="N276" t="n">
+        <v>70</v>
+      </c>
+      <c r="O276" t="n">
+        <v>512</v>
+      </c>
+    </row>
+    <row r="277">
+      <c r="A277" t="inlineStr">
+        <is>
+          <t>2023-08-22 00:15:23</t>
+        </is>
+      </c>
+      <c r="B277" t="n">
+        <v>40</v>
+      </c>
+      <c r="C277" t="n">
+        <v>20</v>
+      </c>
+      <c r="D277" t="n">
+        <v>9</v>
+      </c>
+      <c r="E277" t="n">
+        <v>5</v>
+      </c>
+      <c r="F277" t="n">
+        <v>9</v>
+      </c>
+      <c r="G277" t="n">
+        <v>6</v>
+      </c>
+      <c r="H277" t="n">
+        <v>31</v>
+      </c>
+      <c r="I277" t="n">
+        <v>12</v>
+      </c>
+      <c r="J277" t="n">
+        <v>16</v>
+      </c>
+      <c r="K277" t="n">
+        <v>0.001</v>
+      </c>
+      <c r="L277" t="n">
+        <v>0.01</v>
+      </c>
+      <c r="M277" t="n">
+        <v>0.003</v>
+      </c>
+      <c r="N277" t="n">
+        <v>70</v>
+      </c>
+      <c r="O277" t="n">
+        <v>512</v>
+      </c>
+    </row>
+    <row r="278">
+      <c r="A278" t="inlineStr">
+        <is>
+          <t>2023-08-22 00:15:31</t>
+        </is>
+      </c>
+      <c r="B278" t="n">
+        <v>40</v>
+      </c>
+      <c r="C278" t="n">
+        <v>20</v>
+      </c>
+      <c r="D278" t="n">
+        <v>5</v>
+      </c>
+      <c r="E278" t="n">
+        <v>3</v>
+      </c>
+      <c r="F278" t="n">
+        <v>10</v>
+      </c>
+      <c r="G278" t="n">
+        <v>7</v>
+      </c>
+      <c r="H278" t="n">
+        <v>18</v>
+      </c>
+      <c r="I278" t="n">
+        <v>10</v>
+      </c>
+      <c r="J278" t="n">
+        <v>10</v>
+      </c>
+      <c r="K278" t="n">
+        <v>0.001</v>
+      </c>
+      <c r="L278" t="n">
+        <v>0.01</v>
+      </c>
+      <c r="M278" t="n">
+        <v>0.003</v>
+      </c>
+      <c r="N278" t="n">
+        <v>70</v>
+      </c>
+      <c r="O278" t="n">
+        <v>512</v>
+      </c>
+    </row>
+    <row r="279">
+      <c r="A279" t="inlineStr">
+        <is>
+          <t>2023-08-22 00:15:54</t>
+        </is>
+      </c>
+      <c r="B279" t="n">
+        <v>130</v>
+      </c>
+      <c r="C279" t="n">
+        <v>55</v>
+      </c>
+      <c r="D279" t="n">
+        <v>9</v>
+      </c>
+      <c r="E279" t="n">
+        <v>10</v>
+      </c>
+      <c r="F279" t="n">
+        <v>22</v>
+      </c>
+      <c r="G279" t="n">
+        <v>23</v>
+      </c>
+      <c r="H279" t="n">
+        <v>39</v>
+      </c>
+      <c r="I279" t="n">
+        <v>14</v>
+      </c>
+      <c r="J279" t="n">
+        <v>15</v>
+      </c>
+      <c r="K279" t="n">
+        <v>0.001</v>
+      </c>
+      <c r="L279" t="n">
+        <v>0.01</v>
+      </c>
+      <c r="M279" t="n">
+        <v>0.003</v>
+      </c>
+      <c r="N279" t="n">
+        <v>70</v>
+      </c>
+      <c r="O279" t="n">
+        <v>512</v>
+      </c>
+    </row>
+    <row r="280">
+      <c r="A280" t="inlineStr">
+        <is>
+          <t>2023-08-22 00:16:17</t>
+        </is>
+      </c>
+      <c r="B280" t="n">
+        <v>120</v>
+      </c>
+      <c r="C280" t="n">
+        <v>48</v>
+      </c>
+      <c r="D280" t="n">
+        <v>10</v>
+      </c>
+      <c r="E280" t="n">
+        <v>10</v>
+      </c>
+      <c r="F280" t="n">
+        <v>15</v>
+      </c>
+      <c r="G280" t="n">
+        <v>23</v>
+      </c>
+      <c r="H280" t="n">
+        <v>24</v>
+      </c>
+      <c r="I280" t="n">
+        <v>29</v>
+      </c>
+      <c r="J280" t="n">
+        <v>15</v>
+      </c>
+      <c r="K280" t="n">
+        <v>0.001</v>
+      </c>
+      <c r="L280" t="n">
+        <v>0.01</v>
+      </c>
+      <c r="M280" t="n">
+        <v>0.003</v>
+      </c>
+      <c r="N280" t="n">
+        <v>70</v>
+      </c>
+      <c r="O280" t="n">
+        <v>512</v>
+      </c>
+    </row>
+    <row r="281">
+      <c r="A281" t="inlineStr">
+        <is>
+          <t>2023-08-22 00:16:42</t>
+        </is>
+      </c>
+      <c r="B281" t="n">
+        <v>118</v>
+      </c>
+      <c r="C281" t="n">
+        <v>58</v>
+      </c>
+      <c r="D281" t="n">
+        <v>8</v>
+      </c>
+      <c r="E281" t="n">
+        <v>12</v>
+      </c>
+      <c r="F281" t="n">
+        <v>22</v>
+      </c>
+      <c r="G281" t="n">
+        <v>24</v>
+      </c>
+      <c r="H281" t="n">
+        <v>23</v>
+      </c>
+      <c r="I281" t="n">
+        <v>21</v>
+      </c>
+      <c r="J281" t="n">
+        <v>12</v>
+      </c>
+      <c r="K281" t="n">
+        <v>0.001</v>
+      </c>
+      <c r="L281" t="n">
+        <v>0.01</v>
+      </c>
+      <c r="M281" t="n">
+        <v>0.003</v>
+      </c>
+      <c r="N281" t="n">
+        <v>70</v>
+      </c>
+      <c r="O281" t="n">
+        <v>512</v>
+      </c>
+    </row>
+    <row r="282">
+      <c r="A282" t="inlineStr">
+        <is>
+          <t>2023-08-22 00:25:31</t>
+        </is>
+      </c>
+      <c r="B282" t="n">
+        <v>40</v>
+      </c>
+      <c r="C282" t="n">
+        <v>10</v>
+      </c>
+      <c r="D282" t="n">
+        <v>7</v>
+      </c>
+      <c r="E282" t="n">
+        <v>1</v>
+      </c>
+      <c r="F282" t="n">
+        <v>6</v>
+      </c>
+      <c r="G282" t="n">
+        <v>3</v>
+      </c>
+      <c r="H282" t="n">
+        <v>25</v>
+      </c>
+      <c r="I282" t="n">
+        <v>16</v>
+      </c>
+      <c r="J282" t="n">
+        <v>23</v>
+      </c>
+      <c r="K282" t="n">
+        <v>0.001</v>
+      </c>
+      <c r="L282" t="n">
+        <v>0.01</v>
+      </c>
+      <c r="M282" t="n">
+        <v>0.003</v>
+      </c>
+      <c r="N282" t="n">
+        <v>70</v>
+      </c>
+      <c r="O282" t="n">
+        <v>512</v>
+      </c>
+    </row>
+    <row r="283">
+      <c r="A283" t="inlineStr">
+        <is>
+          <t>2023-08-22 00:25:41</t>
+        </is>
+      </c>
+      <c r="B283" t="n">
+        <v>40</v>
+      </c>
+      <c r="C283" t="n">
+        <v>22</v>
+      </c>
+      <c r="D283" t="n">
+        <v>7</v>
+      </c>
+      <c r="E283" t="n">
+        <v>3</v>
+      </c>
+      <c r="F283" t="n">
+        <v>11</v>
+      </c>
+      <c r="G283" t="n">
+        <v>8</v>
+      </c>
+      <c r="H283" t="n">
+        <v>40</v>
+      </c>
+      <c r="I283" t="n">
+        <v>7</v>
+      </c>
+      <c r="J283" t="n">
+        <v>17</v>
+      </c>
+      <c r="K283" t="n">
+        <v>0.001</v>
+      </c>
+      <c r="L283" t="n">
+        <v>0.01</v>
+      </c>
+      <c r="M283" t="n">
+        <v>0.003</v>
+      </c>
+      <c r="N283" t="n">
+        <v>70</v>
+      </c>
+      <c r="O283" t="n">
+        <v>512</v>
+      </c>
+    </row>
+    <row r="284">
+      <c r="A284" t="inlineStr">
+        <is>
+          <t>2023-08-22 00:26:05</t>
+        </is>
+      </c>
+      <c r="B284" t="n">
+        <v>130</v>
+      </c>
+      <c r="C284" t="n">
+        <v>55</v>
+      </c>
+      <c r="D284" t="n">
+        <v>8</v>
+      </c>
+      <c r="E284" t="n">
+        <v>7</v>
+      </c>
+      <c r="F284" t="n">
+        <v>26</v>
+      </c>
+      <c r="G284" t="n">
+        <v>22</v>
+      </c>
+      <c r="H284" t="n">
+        <v>63</v>
+      </c>
+      <c r="I284" t="n">
+        <v>29</v>
+      </c>
+      <c r="J284" t="n">
+        <v>18</v>
+      </c>
+      <c r="K284" t="n">
+        <v>0.001</v>
+      </c>
+      <c r="L284" t="n">
+        <v>0.01</v>
+      </c>
+      <c r="M284" t="n">
+        <v>0.003</v>
+      </c>
+      <c r="N284" t="n">
+        <v>70</v>
+      </c>
+      <c r="O284" t="n">
+        <v>512</v>
+      </c>
+    </row>
+    <row r="285">
+      <c r="A285" t="inlineStr">
+        <is>
+          <t>2023-08-22 00:26:34</t>
+        </is>
+      </c>
+      <c r="B285" t="n">
+        <v>120</v>
+      </c>
+      <c r="C285" t="n">
+        <v>56</v>
+      </c>
+      <c r="D285" t="n">
+        <v>7</v>
+      </c>
+      <c r="E285" t="n">
+        <v>9</v>
+      </c>
+      <c r="F285" t="n">
+        <v>24</v>
+      </c>
+      <c r="G285" t="n">
+        <v>23</v>
+      </c>
+      <c r="H285" t="n">
+        <v>26</v>
+      </c>
+      <c r="I285" t="n">
+        <v>16</v>
+      </c>
+      <c r="J285" t="n">
+        <v>18</v>
+      </c>
+      <c r="K285" t="n">
+        <v>0.001</v>
+      </c>
+      <c r="L285" t="n">
+        <v>0.01</v>
+      </c>
+      <c r="M285" t="n">
+        <v>0.003</v>
+      </c>
+      <c r="N285" t="n">
+        <v>70</v>
+      </c>
+      <c r="O285" t="n">
+        <v>512</v>
+      </c>
+    </row>
+    <row r="286">
+      <c r="A286" t="inlineStr">
+        <is>
+          <t>2023-08-22 00:26:57</t>
+        </is>
+      </c>
+      <c r="B286" t="n">
+        <v>118</v>
+      </c>
+      <c r="C286" t="n">
+        <v>63</v>
+      </c>
+      <c r="D286" t="n">
+        <v>6</v>
+      </c>
+      <c r="E286" t="n">
+        <v>14</v>
+      </c>
+      <c r="F286" t="n">
+        <v>23</v>
+      </c>
+      <c r="G286" t="n">
+        <v>26</v>
+      </c>
+      <c r="H286" t="n">
+        <v>18</v>
+      </c>
+      <c r="I286" t="n">
+        <v>31</v>
+      </c>
+      <c r="J286" t="n">
+        <v>9</v>
+      </c>
+      <c r="K286" t="n">
+        <v>0.001</v>
+      </c>
+      <c r="L286" t="n">
+        <v>0.01</v>
+      </c>
+      <c r="M286" t="n">
+        <v>0.003</v>
+      </c>
+      <c r="N286" t="n">
+        <v>70</v>
+      </c>
+      <c r="O286" t="n">
+        <v>512</v>
+      </c>
+    </row>
+    <row r="287">
+      <c r="A287" t="inlineStr">
+        <is>
+          <t>2023-08-22 00:32:05</t>
+        </is>
+      </c>
+      <c r="B287" t="n">
+        <v>40</v>
+      </c>
+      <c r="C287" t="n">
+        <v>15</v>
+      </c>
+      <c r="D287" t="n">
+        <v>7</v>
+      </c>
+      <c r="E287" t="n">
+        <v>1</v>
+      </c>
+      <c r="F287" t="n">
+        <v>5</v>
+      </c>
+      <c r="G287" t="n">
+        <v>9</v>
+      </c>
+      <c r="H287" t="n">
+        <v>25</v>
+      </c>
+      <c r="I287" t="n">
+        <v>13</v>
+      </c>
+      <c r="J287" t="n">
+        <v>12</v>
+      </c>
+      <c r="K287" t="n">
+        <v>0.001</v>
+      </c>
+      <c r="L287" t="n">
+        <v>0.01</v>
+      </c>
+      <c r="M287" t="n">
+        <v>0.003</v>
+      </c>
+      <c r="N287" t="n">
+        <v>75</v>
+      </c>
+      <c r="O287" t="n">
+        <v>512</v>
+      </c>
+    </row>
+    <row r="288">
+      <c r="A288" t="inlineStr">
+        <is>
+          <t>2023-08-22 00:32:15</t>
+        </is>
+      </c>
+      <c r="B288" t="n">
+        <v>40</v>
+      </c>
+      <c r="C288" t="n">
+        <v>18</v>
+      </c>
+      <c r="D288" t="n">
+        <v>8</v>
+      </c>
+      <c r="E288" t="n">
+        <v>5</v>
+      </c>
+      <c r="F288" t="n">
+        <v>7</v>
+      </c>
+      <c r="G288" t="n">
+        <v>6</v>
+      </c>
+      <c r="H288" t="n">
+        <v>21</v>
+      </c>
+      <c r="I288" t="n">
+        <v>10</v>
+      </c>
+      <c r="J288" t="n">
+        <v>19</v>
+      </c>
+      <c r="K288" t="n">
+        <v>0.001</v>
+      </c>
+      <c r="L288" t="n">
+        <v>0.01</v>
+      </c>
+      <c r="M288" t="n">
+        <v>0.003</v>
+      </c>
+      <c r="N288" t="n">
+        <v>75</v>
+      </c>
+      <c r="O288" t="n">
+        <v>512</v>
+      </c>
+    </row>
+    <row r="289">
+      <c r="A289" t="inlineStr">
+        <is>
+          <t>2023-08-22 00:32:41</t>
+        </is>
+      </c>
+      <c r="B289" t="n">
+        <v>130</v>
+      </c>
+      <c r="C289" t="n">
+        <v>51</v>
+      </c>
+      <c r="D289" t="n">
+        <v>10</v>
+      </c>
+      <c r="E289" t="n">
+        <v>8</v>
+      </c>
+      <c r="F289" t="n">
+        <v>24</v>
+      </c>
+      <c r="G289" t="n">
+        <v>19</v>
+      </c>
+      <c r="H289" t="n">
+        <v>31</v>
+      </c>
+      <c r="I289" t="n">
+        <v>16</v>
+      </c>
+      <c r="J289" t="n">
+        <v>26</v>
+      </c>
+      <c r="K289" t="n">
+        <v>0.001</v>
+      </c>
+      <c r="L289" t="n">
+        <v>0.01</v>
+      </c>
+      <c r="M289" t="n">
+        <v>0.003</v>
+      </c>
+      <c r="N289" t="n">
+        <v>75</v>
+      </c>
+      <c r="O289" t="n">
+        <v>512</v>
+      </c>
+    </row>
+    <row r="290">
+      <c r="A290" t="inlineStr">
+        <is>
+          <t>2023-08-22 00:33:05</t>
+        </is>
+      </c>
+      <c r="B290" t="n">
+        <v>120</v>
+      </c>
+      <c r="C290" t="n">
+        <v>45</v>
+      </c>
+      <c r="D290" t="n">
+        <v>14</v>
+      </c>
+      <c r="E290" t="n">
+        <v>12</v>
+      </c>
+      <c r="F290" t="n">
+        <v>17</v>
+      </c>
+      <c r="G290" t="n">
+        <v>16</v>
+      </c>
+      <c r="H290" t="n">
+        <v>26</v>
+      </c>
+      <c r="I290" t="n">
+        <v>26</v>
+      </c>
+      <c r="J290" t="n">
+        <v>27</v>
+      </c>
+      <c r="K290" t="n">
+        <v>0.001</v>
+      </c>
+      <c r="L290" t="n">
+        <v>0.01</v>
+      </c>
+      <c r="M290" t="n">
+        <v>0.003</v>
+      </c>
+      <c r="N290" t="n">
+        <v>75</v>
+      </c>
+      <c r="O290" t="n">
+        <v>512</v>
+      </c>
+    </row>
+    <row r="291">
+      <c r="A291" t="inlineStr">
+        <is>
+          <t>2023-08-22 00:33:31</t>
+        </is>
+      </c>
+      <c r="B291" t="n">
+        <v>118</v>
+      </c>
+      <c r="C291" t="n">
+        <v>54</v>
+      </c>
+      <c r="D291" t="n">
+        <v>9</v>
+      </c>
+      <c r="E291" t="n">
+        <v>7</v>
+      </c>
+      <c r="F291" t="n">
+        <v>26</v>
+      </c>
+      <c r="G291" t="n">
+        <v>21</v>
+      </c>
+      <c r="H291" t="n">
+        <v>33</v>
+      </c>
+      <c r="I291" t="n">
+        <v>18</v>
+      </c>
+      <c r="J291" t="n">
+        <v>29</v>
+      </c>
+      <c r="K291" t="n">
+        <v>0.001</v>
+      </c>
+      <c r="L291" t="n">
+        <v>0.01</v>
+      </c>
+      <c r="M291" t="n">
+        <v>0.003</v>
+      </c>
+      <c r="N291" t="n">
+        <v>75</v>
+      </c>
+      <c r="O291" t="n">
+        <v>512</v>
+      </c>
+    </row>
+    <row r="292">
+      <c r="A292" t="inlineStr">
+        <is>
+          <t>2023-08-22 08:15:29</t>
+        </is>
+      </c>
+      <c r="B292" t="n">
+        <v>40</v>
+      </c>
+      <c r="C292" t="n">
+        <v>21</v>
+      </c>
+      <c r="D292" t="n">
+        <v>4</v>
+      </c>
+      <c r="E292" t="n">
+        <v>3</v>
+      </c>
+      <c r="F292" t="n">
+        <v>12</v>
+      </c>
+      <c r="G292" t="n">
+        <v>6</v>
+      </c>
+      <c r="H292" t="n">
+        <v>25</v>
+      </c>
+      <c r="I292" t="n">
+        <v>9</v>
+      </c>
+      <c r="J292" t="n">
+        <v>18</v>
+      </c>
+      <c r="K292" t="n">
+        <v>0.002</v>
+      </c>
+      <c r="L292" t="n">
+        <v>0.01</v>
+      </c>
+      <c r="M292" t="n">
+        <v>0.003</v>
+      </c>
+      <c r="N292" t="n">
+        <v>70</v>
+      </c>
+      <c r="O292" t="n">
+        <v>512</v>
+      </c>
+    </row>
+    <row r="293">
+      <c r="A293" t="inlineStr">
+        <is>
+          <t>2023-08-22 08:15:37</t>
+        </is>
+      </c>
+      <c r="B293" t="n">
+        <v>40</v>
+      </c>
+      <c r="C293" t="n">
+        <v>21</v>
+      </c>
+      <c r="D293" t="n">
+        <v>5</v>
+      </c>
+      <c r="E293" t="n">
+        <v>1</v>
+      </c>
+      <c r="F293" t="n">
+        <v>12</v>
+      </c>
+      <c r="G293" t="n">
+        <v>8</v>
+      </c>
+      <c r="H293" t="n">
+        <v>44</v>
+      </c>
+      <c r="I293" t="n">
+        <v>11</v>
+      </c>
+      <c r="J293" t="n">
+        <v>17</v>
+      </c>
+      <c r="K293" t="n">
+        <v>0.002</v>
+      </c>
+      <c r="L293" t="n">
+        <v>0.01</v>
+      </c>
+      <c r="M293" t="n">
+        <v>0.003</v>
+      </c>
+      <c r="N293" t="n">
+        <v>70</v>
+      </c>
+      <c r="O293" t="n">
+        <v>512</v>
+      </c>
+    </row>
+    <row r="294">
+      <c r="A294" t="inlineStr">
+        <is>
+          <t>2023-08-22 08:15:54</t>
+        </is>
+      </c>
+      <c r="B294" t="n">
+        <v>130</v>
+      </c>
+      <c r="C294" t="n">
+        <v>57</v>
+      </c>
+      <c r="D294" t="n">
+        <v>12</v>
+      </c>
+      <c r="E294" t="n">
+        <v>9</v>
+      </c>
+      <c r="F294" t="n">
+        <v>25</v>
+      </c>
+      <c r="G294" t="n">
+        <v>23</v>
+      </c>
+      <c r="H294" t="n">
+        <v>34</v>
+      </c>
+      <c r="I294" t="n">
+        <v>17</v>
+      </c>
+      <c r="J294" t="n">
+        <v>16</v>
+      </c>
+      <c r="K294" t="n">
+        <v>0.002</v>
+      </c>
+      <c r="L294" t="n">
+        <v>0.01</v>
+      </c>
+      <c r="M294" t="n">
+        <v>0.003</v>
+      </c>
+      <c r="N294" t="n">
+        <v>70</v>
+      </c>
+      <c r="O294" t="n">
+        <v>512</v>
+      </c>
+    </row>
+    <row r="295">
+      <c r="A295" t="inlineStr">
+        <is>
+          <t>2023-08-22 08:16:10</t>
+        </is>
+      </c>
+      <c r="B295" t="n">
+        <v>120</v>
+      </c>
+      <c r="C295" t="n">
+        <v>54</v>
+      </c>
+      <c r="D295" t="n">
+        <v>9</v>
+      </c>
+      <c r="E295" t="n">
+        <v>10</v>
+      </c>
+      <c r="F295" t="n">
+        <v>22</v>
+      </c>
+      <c r="G295" t="n">
+        <v>22</v>
+      </c>
+      <c r="H295" t="n">
+        <v>27</v>
+      </c>
+      <c r="I295" t="n">
+        <v>16</v>
+      </c>
+      <c r="J295" t="n">
+        <v>20</v>
+      </c>
+      <c r="K295" t="n">
+        <v>0.002</v>
+      </c>
+      <c r="L295" t="n">
+        <v>0.01</v>
+      </c>
+      <c r="M295" t="n">
+        <v>0.003</v>
+      </c>
+      <c r="N295" t="n">
+        <v>70</v>
+      </c>
+      <c r="O295" t="n">
+        <v>512</v>
+      </c>
+    </row>
+    <row r="296">
+      <c r="A296" t="inlineStr">
+        <is>
+          <t>2023-08-22 08:16:25</t>
+        </is>
+      </c>
+      <c r="B296" t="n">
+        <v>118</v>
+      </c>
+      <c r="C296" t="n">
+        <v>42</v>
+      </c>
+      <c r="D296" t="n">
+        <v>16</v>
+      </c>
+      <c r="E296" t="n">
+        <v>10</v>
+      </c>
+      <c r="F296" t="n">
+        <v>13</v>
+      </c>
+      <c r="G296" t="n">
+        <v>19</v>
+      </c>
+      <c r="H296" t="n">
+        <v>31</v>
+      </c>
+      <c r="I296" t="n">
+        <v>20</v>
+      </c>
+      <c r="J296" t="n">
+        <v>18</v>
+      </c>
+      <c r="K296" t="n">
+        <v>0.002</v>
+      </c>
+      <c r="L296" t="n">
+        <v>0.01</v>
+      </c>
+      <c r="M296" t="n">
+        <v>0.003</v>
+      </c>
+      <c r="N296" t="n">
+        <v>70</v>
+      </c>
+      <c r="O296" t="n">
+        <v>512</v>
+      </c>
+    </row>
+    <row r="297">
+      <c r="A297" t="inlineStr">
+        <is>
+          <t>2023-08-22 08:20:49</t>
+        </is>
+      </c>
+      <c r="B297" t="n">
+        <v>40</v>
+      </c>
+      <c r="C297" t="n">
+        <v>10</v>
+      </c>
+      <c r="D297" t="n">
+        <v>15</v>
+      </c>
+      <c r="E297" t="n">
+        <v>3</v>
+      </c>
+      <c r="F297" t="n">
+        <v>4</v>
+      </c>
+      <c r="G297" t="n">
+        <v>3</v>
+      </c>
+      <c r="H297" t="n">
+        <v>23</v>
+      </c>
+      <c r="I297" t="n">
+        <v>25</v>
+      </c>
+      <c r="J297" t="n">
+        <v>21</v>
+      </c>
+      <c r="K297" t="n">
+        <v>0.001</v>
+      </c>
+      <c r="L297" t="n">
+        <v>0.01</v>
+      </c>
+      <c r="M297" t="n">
+        <v>0.003</v>
+      </c>
+      <c r="N297" t="n">
+        <v>70</v>
+      </c>
+      <c r="O297" t="n">
+        <v>512</v>
+      </c>
+    </row>
+    <row r="298">
+      <c r="A298" t="inlineStr">
+        <is>
+          <t>2023-08-22 08:21:10</t>
+        </is>
+      </c>
+      <c r="B298" t="n">
+        <v>40</v>
+      </c>
+      <c r="C298" t="n">
+        <v>24</v>
+      </c>
+      <c r="D298" t="n">
+        <v>5</v>
+      </c>
+      <c r="E298" t="n">
+        <v>7</v>
+      </c>
+      <c r="F298" t="n">
+        <v>9</v>
+      </c>
+      <c r="G298" t="n">
+        <v>8</v>
+      </c>
+      <c r="H298" t="n">
+        <v>9</v>
+      </c>
+      <c r="I298" t="n">
+        <v>10</v>
+      </c>
+      <c r="J298" t="n">
+        <v>17</v>
+      </c>
+      <c r="K298" t="n">
+        <v>0.001</v>
+      </c>
+      <c r="L298" t="n">
+        <v>0.01</v>
+      </c>
+      <c r="M298" t="n">
+        <v>0.003</v>
+      </c>
+      <c r="N298" t="n">
+        <v>70</v>
+      </c>
+      <c r="O298" t="n">
+        <v>512</v>
+      </c>
+    </row>
+    <row r="299">
+      <c r="A299" t="inlineStr">
+        <is>
+          <t>2023-08-22 08:21:41</t>
+        </is>
+      </c>
+      <c r="B299" t="n">
+        <v>130</v>
+      </c>
+      <c r="C299" t="n">
+        <v>63</v>
+      </c>
+      <c r="D299" t="n">
+        <v>7</v>
+      </c>
+      <c r="E299" t="n">
+        <v>14</v>
+      </c>
+      <c r="F299" t="n">
+        <v>26</v>
+      </c>
+      <c r="G299" t="n">
+        <v>23</v>
+      </c>
+      <c r="H299" t="n">
+        <v>28</v>
+      </c>
+      <c r="I299" t="n">
+        <v>16</v>
+      </c>
+      <c r="J299" t="n">
+        <v>21</v>
+      </c>
+      <c r="K299" t="n">
+        <v>0.001</v>
+      </c>
+      <c r="L299" t="n">
+        <v>0.01</v>
+      </c>
+      <c r="M299" t="n">
+        <v>0.003</v>
+      </c>
+      <c r="N299" t="n">
+        <v>70</v>
+      </c>
+      <c r="O299" t="n">
+        <v>512</v>
+      </c>
+    </row>
+    <row r="300">
+      <c r="A300" t="inlineStr">
+        <is>
+          <t>2023-08-22 08:22:20</t>
+        </is>
+      </c>
+      <c r="B300" t="n">
+        <v>120</v>
+      </c>
+      <c r="C300" t="n">
+        <v>59</v>
+      </c>
+      <c r="D300" t="n">
+        <v>11</v>
+      </c>
+      <c r="E300" t="n">
+        <v>10</v>
+      </c>
+      <c r="F300" t="n">
+        <v>22</v>
+      </c>
+      <c r="G300" t="n">
+        <v>27</v>
+      </c>
+      <c r="H300" t="n">
+        <v>37</v>
+      </c>
+      <c r="I300" t="n">
+        <v>16</v>
+      </c>
+      <c r="J300" t="n">
+        <v>23</v>
+      </c>
+      <c r="K300" t="n">
+        <v>0.001</v>
+      </c>
+      <c r="L300" t="n">
+        <v>0.01</v>
+      </c>
+      <c r="M300" t="n">
+        <v>0.003</v>
+      </c>
+      <c r="N300" t="n">
+        <v>70</v>
+      </c>
+      <c r="O300" t="n">
+        <v>512</v>
+      </c>
+    </row>
+    <row r="301">
+      <c r="A301" t="inlineStr">
+        <is>
+          <t>2023-08-22 08:22:57</t>
+        </is>
+      </c>
+      <c r="B301" t="n">
+        <v>118</v>
+      </c>
+      <c r="C301" t="n">
+        <v>54</v>
+      </c>
+      <c r="D301" t="n">
+        <v>8</v>
+      </c>
+      <c r="E301" t="n">
+        <v>7</v>
+      </c>
+      <c r="F301" t="n">
+        <v>21</v>
+      </c>
+      <c r="G301" t="n">
+        <v>26</v>
+      </c>
+      <c r="H301" t="n">
+        <v>47</v>
+      </c>
+      <c r="I301" t="n">
+        <v>25</v>
+      </c>
+      <c r="J301" t="n">
+        <v>9</v>
+      </c>
+      <c r="K301" t="n">
+        <v>0.001</v>
+      </c>
+      <c r="L301" t="n">
+        <v>0.01</v>
+      </c>
+      <c r="M301" t="n">
+        <v>0.003</v>
+      </c>
+      <c r="N301" t="n">
+        <v>70</v>
+      </c>
+      <c r="O301" t="n">
+        <v>512</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
cambios de nuevos numeros agregados
</commit_message>
<xml_diff>
--- a/Reportes.xlsx
+++ b/Reportes.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:R461"/>
+  <dimension ref="A1:R463"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -26393,6 +26393,122 @@
         <v>0.07692307692307693</v>
       </c>
     </row>
+    <row r="462">
+      <c r="A462" t="inlineStr">
+        <is>
+          <t>2023-11-23 21:26:51</t>
+        </is>
+      </c>
+      <c r="B462" t="n">
+        <v>12</v>
+      </c>
+      <c r="C462" t="n">
+        <v>3</v>
+      </c>
+      <c r="D462" t="n">
+        <v>4</v>
+      </c>
+      <c r="E462" t="n">
+        <v>0</v>
+      </c>
+      <c r="F462" t="n">
+        <v>0</v>
+      </c>
+      <c r="G462" t="n">
+        <v>3</v>
+      </c>
+      <c r="H462" t="n">
+        <v>13</v>
+      </c>
+      <c r="I462" t="n">
+        <v>13</v>
+      </c>
+      <c r="J462" t="n">
+        <v>4</v>
+      </c>
+      <c r="K462" t="n">
+        <v>0.001</v>
+      </c>
+      <c r="L462" t="n">
+        <v>0.01</v>
+      </c>
+      <c r="M462" t="n">
+        <v>0.003</v>
+      </c>
+      <c r="N462" t="n">
+        <v>100</v>
+      </c>
+      <c r="O462" t="n">
+        <v>512</v>
+      </c>
+      <c r="P462" t="n">
+        <v>10</v>
+      </c>
+      <c r="Q462" t="n">
+        <v>7</v>
+      </c>
+      <c r="R462" t="n">
+        <v>0.25</v>
+      </c>
+    </row>
+    <row r="463">
+      <c r="A463" t="inlineStr">
+        <is>
+          <t>2023-11-23 23:12:11</t>
+        </is>
+      </c>
+      <c r="B463" t="n">
+        <v>35</v>
+      </c>
+      <c r="C463" t="n">
+        <v>6</v>
+      </c>
+      <c r="D463" t="n">
+        <v>11</v>
+      </c>
+      <c r="E463" t="n">
+        <v>2</v>
+      </c>
+      <c r="F463" t="n">
+        <v>4</v>
+      </c>
+      <c r="G463" t="n">
+        <v>0</v>
+      </c>
+      <c r="H463" t="n">
+        <v>15</v>
+      </c>
+      <c r="I463" t="n">
+        <v>12</v>
+      </c>
+      <c r="J463" t="n">
+        <v>36</v>
+      </c>
+      <c r="K463" t="n">
+        <v>0.001</v>
+      </c>
+      <c r="L463" t="n">
+        <v>0.01</v>
+      </c>
+      <c r="M463" t="n">
+        <v>0.003</v>
+      </c>
+      <c r="N463" t="n">
+        <v>100</v>
+      </c>
+      <c r="O463" t="n">
+        <v>512</v>
+      </c>
+      <c r="P463" t="n">
+        <v>10</v>
+      </c>
+      <c r="Q463" t="n">
+        <v>7</v>
+      </c>
+      <c r="R463" t="n">
+        <v>0.1714285714285714</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
confirmar los cambios en datos
</commit_message>
<xml_diff>
--- a/Reportes.xlsx
+++ b/Reportes.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:R463"/>
+  <dimension ref="A1:R469"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -26509,6 +26509,354 @@
         <v>0.1714285714285714</v>
       </c>
     </row>
+    <row r="464">
+      <c r="A464" t="inlineStr">
+        <is>
+          <t>2023-11-25 00:55:53</t>
+        </is>
+      </c>
+      <c r="B464" t="n">
+        <v>21</v>
+      </c>
+      <c r="C464" t="n">
+        <v>5</v>
+      </c>
+      <c r="D464" t="n">
+        <v>12</v>
+      </c>
+      <c r="E464" t="n">
+        <v>0</v>
+      </c>
+      <c r="F464" t="n">
+        <v>3</v>
+      </c>
+      <c r="G464" t="n">
+        <v>2</v>
+      </c>
+      <c r="H464" t="n">
+        <v>23</v>
+      </c>
+      <c r="I464" t="n">
+        <v>20</v>
+      </c>
+      <c r="J464" t="n">
+        <v>15</v>
+      </c>
+      <c r="K464" t="n">
+        <v>0.001</v>
+      </c>
+      <c r="L464" t="n">
+        <v>0.01</v>
+      </c>
+      <c r="M464" t="n">
+        <v>0.003</v>
+      </c>
+      <c r="N464" t="n">
+        <v>100</v>
+      </c>
+      <c r="O464" t="n">
+        <v>512</v>
+      </c>
+      <c r="P464" t="n">
+        <v>10</v>
+      </c>
+      <c r="Q464" t="n">
+        <v>7</v>
+      </c>
+      <c r="R464" t="n">
+        <v>0.2380952380952381</v>
+      </c>
+    </row>
+    <row r="465">
+      <c r="A465" t="inlineStr">
+        <is>
+          <t>2023-11-25 11:06:27</t>
+        </is>
+      </c>
+      <c r="B465" t="n">
+        <v>56</v>
+      </c>
+      <c r="C465" t="n">
+        <v>7</v>
+      </c>
+      <c r="D465" t="n">
+        <v>21</v>
+      </c>
+      <c r="E465" t="n">
+        <v>1</v>
+      </c>
+      <c r="F465" t="n">
+        <v>5</v>
+      </c>
+      <c r="G465" t="n">
+        <v>1</v>
+      </c>
+      <c r="H465" t="n">
+        <v>41</v>
+      </c>
+      <c r="I465" t="n">
+        <v>21</v>
+      </c>
+      <c r="J465" t="n">
+        <v>36</v>
+      </c>
+      <c r="K465" t="n">
+        <v>0.001</v>
+      </c>
+      <c r="L465" t="n">
+        <v>0.01</v>
+      </c>
+      <c r="M465" t="n">
+        <v>0.003</v>
+      </c>
+      <c r="N465" t="n">
+        <v>100</v>
+      </c>
+      <c r="O465" t="n">
+        <v>512</v>
+      </c>
+      <c r="P465" t="n">
+        <v>10</v>
+      </c>
+      <c r="Q465" t="n">
+        <v>7</v>
+      </c>
+      <c r="R465" t="n">
+        <v>0.125</v>
+      </c>
+    </row>
+    <row r="466">
+      <c r="A466" t="inlineStr">
+        <is>
+          <t>2023-11-25 11:44:58</t>
+        </is>
+      </c>
+      <c r="B466" t="n">
+        <v>98</v>
+      </c>
+      <c r="C466" t="n">
+        <v>13</v>
+      </c>
+      <c r="D466" t="n">
+        <v>23</v>
+      </c>
+      <c r="E466" t="n">
+        <v>3</v>
+      </c>
+      <c r="F466" t="n">
+        <v>3</v>
+      </c>
+      <c r="G466" t="n">
+        <v>7</v>
+      </c>
+      <c r="H466" t="n">
+        <v>44</v>
+      </c>
+      <c r="I466" t="n">
+        <v>58</v>
+      </c>
+      <c r="J466" t="n">
+        <v>23</v>
+      </c>
+      <c r="K466" t="n">
+        <v>0.001</v>
+      </c>
+      <c r="L466" t="n">
+        <v>0.01</v>
+      </c>
+      <c r="M466" t="n">
+        <v>0.003</v>
+      </c>
+      <c r="N466" t="n">
+        <v>100</v>
+      </c>
+      <c r="O466" t="n">
+        <v>512</v>
+      </c>
+      <c r="P466" t="n">
+        <v>10</v>
+      </c>
+      <c r="Q466" t="n">
+        <v>7</v>
+      </c>
+      <c r="R466" t="n">
+        <v>0.1326530612244898</v>
+      </c>
+    </row>
+    <row r="467">
+      <c r="A467" t="inlineStr">
+        <is>
+          <t>2023-11-25 19:07:44</t>
+        </is>
+      </c>
+      <c r="B467" t="n">
+        <v>14</v>
+      </c>
+      <c r="C467" t="n">
+        <v>0</v>
+      </c>
+      <c r="D467" t="n">
+        <v>14</v>
+      </c>
+      <c r="E467" t="n">
+        <v>0</v>
+      </c>
+      <c r="F467" t="n">
+        <v>0</v>
+      </c>
+      <c r="G467" t="n">
+        <v>0</v>
+      </c>
+      <c r="H467" t="n">
+        <v>14</v>
+      </c>
+      <c r="I467" t="n">
+        <v>14</v>
+      </c>
+      <c r="J467" t="n">
+        <v>14</v>
+      </c>
+      <c r="K467" t="n">
+        <v>0.001</v>
+      </c>
+      <c r="L467" t="n">
+        <v>0.01</v>
+      </c>
+      <c r="M467" t="n">
+        <v>0.003</v>
+      </c>
+      <c r="N467" t="n">
+        <v>100</v>
+      </c>
+      <c r="O467" t="n">
+        <v>512</v>
+      </c>
+      <c r="P467" t="n">
+        <v>10</v>
+      </c>
+      <c r="Q467" t="n">
+        <v>7</v>
+      </c>
+      <c r="R467" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="468">
+      <c r="A468" t="inlineStr">
+        <is>
+          <t>2023-11-25 19:19:02</t>
+        </is>
+      </c>
+      <c r="B468" t="n">
+        <v>63</v>
+      </c>
+      <c r="C468" t="n">
+        <v>7</v>
+      </c>
+      <c r="D468" t="n">
+        <v>24</v>
+      </c>
+      <c r="E468" t="n">
+        <v>1</v>
+      </c>
+      <c r="F468" t="n">
+        <v>3</v>
+      </c>
+      <c r="G468" t="n">
+        <v>3</v>
+      </c>
+      <c r="H468" t="n">
+        <v>52</v>
+      </c>
+      <c r="I468" t="n">
+        <v>46</v>
+      </c>
+      <c r="J468" t="n">
+        <v>24</v>
+      </c>
+      <c r="K468" t="n">
+        <v>0.001</v>
+      </c>
+      <c r="L468" t="n">
+        <v>0.01</v>
+      </c>
+      <c r="M468" t="n">
+        <v>0.003</v>
+      </c>
+      <c r="N468" t="n">
+        <v>100</v>
+      </c>
+      <c r="O468" t="n">
+        <v>512</v>
+      </c>
+      <c r="P468" t="n">
+        <v>10</v>
+      </c>
+      <c r="Q468" t="n">
+        <v>7</v>
+      </c>
+      <c r="R468" t="n">
+        <v>0.1111111111111111</v>
+      </c>
+    </row>
+    <row r="469">
+      <c r="A469" t="inlineStr">
+        <is>
+          <t>2023-11-25 20:35:36</t>
+        </is>
+      </c>
+      <c r="B469" t="n">
+        <v>31</v>
+      </c>
+      <c r="C469" t="n">
+        <v>5</v>
+      </c>
+      <c r="D469" t="n">
+        <v>8</v>
+      </c>
+      <c r="E469" t="n">
+        <v>1</v>
+      </c>
+      <c r="F469" t="n">
+        <v>4</v>
+      </c>
+      <c r="G469" t="n">
+        <v>0</v>
+      </c>
+      <c r="H469" t="n">
+        <v>24</v>
+      </c>
+      <c r="I469" t="n">
+        <v>12</v>
+      </c>
+      <c r="J469" t="n">
+        <v>31</v>
+      </c>
+      <c r="K469" t="n">
+        <v>0.001</v>
+      </c>
+      <c r="L469" t="n">
+        <v>0.01</v>
+      </c>
+      <c r="M469" t="n">
+        <v>0.003</v>
+      </c>
+      <c r="N469" t="n">
+        <v>100</v>
+      </c>
+      <c r="O469" t="n">
+        <v>512</v>
+      </c>
+      <c r="P469" t="n">
+        <v>10</v>
+      </c>
+      <c r="Q469" t="n">
+        <v>7</v>
+      </c>
+      <c r="R469" t="n">
+        <v>0.1612903225806452</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
confirmar se tomo como parametro de la ruleta 3000 tiros aleatorios
</commit_message>
<xml_diff>
--- a/Reportes.xlsx
+++ b/Reportes.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:R216"/>
+  <dimension ref="A1:R218"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -12995,6 +12995,122 @@
         <v>0.1627906976744186</v>
       </c>
     </row>
+    <row r="217">
+      <c r="A217" t="inlineStr">
+        <is>
+          <t>2023-11-29 02:02:36</t>
+        </is>
+      </c>
+      <c r="B217" t="n">
+        <v>18</v>
+      </c>
+      <c r="C217" t="n">
+        <v>1</v>
+      </c>
+      <c r="D217" t="n">
+        <v>13</v>
+      </c>
+      <c r="E217" t="n">
+        <v>0</v>
+      </c>
+      <c r="F217" t="n">
+        <v>0</v>
+      </c>
+      <c r="G217" t="n">
+        <v>1</v>
+      </c>
+      <c r="H217" t="n">
+        <v>18</v>
+      </c>
+      <c r="I217" t="n">
+        <v>18</v>
+      </c>
+      <c r="J217" t="n">
+        <v>13</v>
+      </c>
+      <c r="K217" t="n">
+        <v>0.001</v>
+      </c>
+      <c r="L217" t="n">
+        <v>0.01</v>
+      </c>
+      <c r="M217" t="n">
+        <v>0.003</v>
+      </c>
+      <c r="N217" t="n">
+        <v>100</v>
+      </c>
+      <c r="O217" t="n">
+        <v>512</v>
+      </c>
+      <c r="P217" t="n">
+        <v>10</v>
+      </c>
+      <c r="Q217" t="n">
+        <v>7</v>
+      </c>
+      <c r="R217" t="n">
+        <v>0.05555555555555555</v>
+      </c>
+    </row>
+    <row r="218">
+      <c r="A218" t="inlineStr">
+        <is>
+          <t>2023-11-29 20:52:15</t>
+        </is>
+      </c>
+      <c r="B218" t="n">
+        <v>47</v>
+      </c>
+      <c r="C218" t="n">
+        <v>10</v>
+      </c>
+      <c r="D218" t="n">
+        <v>11</v>
+      </c>
+      <c r="E218" t="n">
+        <v>0</v>
+      </c>
+      <c r="F218" t="n">
+        <v>4</v>
+      </c>
+      <c r="G218" t="n">
+        <v>6</v>
+      </c>
+      <c r="H218" t="n">
+        <v>48</v>
+      </c>
+      <c r="I218" t="n">
+        <v>20</v>
+      </c>
+      <c r="J218" t="n">
+        <v>24</v>
+      </c>
+      <c r="K218" t="n">
+        <v>0.001</v>
+      </c>
+      <c r="L218" t="n">
+        <v>0.01</v>
+      </c>
+      <c r="M218" t="n">
+        <v>0.003</v>
+      </c>
+      <c r="N218" t="n">
+        <v>100</v>
+      </c>
+      <c r="O218" t="n">
+        <v>512</v>
+      </c>
+      <c r="P218" t="n">
+        <v>10</v>
+      </c>
+      <c r="Q218" t="n">
+        <v>7</v>
+      </c>
+      <c r="R218" t="n">
+        <v>0.2127659574468085</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
fijarse si sale de dos numero de los vecinos ?
</commit_message>
<xml_diff>
--- a/Reportes.xlsx
+++ b/Reportes.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:R218"/>
+  <dimension ref="A1:R219"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -13111,6 +13111,64 @@
         <v>0.2127659574468085</v>
       </c>
     </row>
+    <row r="219">
+      <c r="A219" t="inlineStr">
+        <is>
+          <t>2023-11-29 22:02:29</t>
+        </is>
+      </c>
+      <c r="B219" t="n">
+        <v>27</v>
+      </c>
+      <c r="C219" t="n">
+        <v>5</v>
+      </c>
+      <c r="D219" t="n">
+        <v>11</v>
+      </c>
+      <c r="E219" t="n">
+        <v>2</v>
+      </c>
+      <c r="F219" t="n">
+        <v>0</v>
+      </c>
+      <c r="G219" t="n">
+        <v>3</v>
+      </c>
+      <c r="H219" t="n">
+        <v>18</v>
+      </c>
+      <c r="I219" t="n">
+        <v>27</v>
+      </c>
+      <c r="J219" t="n">
+        <v>11</v>
+      </c>
+      <c r="K219" t="n">
+        <v>0.001</v>
+      </c>
+      <c r="L219" t="n">
+        <v>0.01</v>
+      </c>
+      <c r="M219" t="n">
+        <v>0.003</v>
+      </c>
+      <c r="N219" t="n">
+        <v>100</v>
+      </c>
+      <c r="O219" t="n">
+        <v>512</v>
+      </c>
+      <c r="P219" t="n">
+        <v>10</v>
+      </c>
+      <c r="Q219" t="n">
+        <v>7</v>
+      </c>
+      <c r="R219" t="n">
+        <v>0.1851851851851852</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
se necesita cambiar la formula para que se contee
</commit_message>
<xml_diff>
--- a/Reportes.xlsx
+++ b/Reportes.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:R219"/>
+  <dimension ref="A1:R228"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -13169,6 +13169,528 @@
         <v>0.1851851851851852</v>
       </c>
     </row>
+    <row r="220">
+      <c r="A220" t="inlineStr">
+        <is>
+          <t>2023-11-30 20:34:36</t>
+        </is>
+      </c>
+      <c r="B220" t="n">
+        <v>9</v>
+      </c>
+      <c r="C220" t="n">
+        <v>1</v>
+      </c>
+      <c r="D220" t="n">
+        <v>7</v>
+      </c>
+      <c r="E220" t="n">
+        <v>1</v>
+      </c>
+      <c r="F220" t="n">
+        <v>0</v>
+      </c>
+      <c r="G220" t="n">
+        <v>0</v>
+      </c>
+      <c r="H220" t="n">
+        <v>7</v>
+      </c>
+      <c r="I220" t="n">
+        <v>10</v>
+      </c>
+      <c r="J220" t="n">
+        <v>10</v>
+      </c>
+      <c r="K220" t="n">
+        <v>0.001</v>
+      </c>
+      <c r="L220" t="n">
+        <v>0.01</v>
+      </c>
+      <c r="M220" t="n">
+        <v>0.003</v>
+      </c>
+      <c r="N220" t="n">
+        <v>100</v>
+      </c>
+      <c r="O220" t="n">
+        <v>512</v>
+      </c>
+      <c r="P220" t="n">
+        <v>10</v>
+      </c>
+      <c r="Q220" t="n">
+        <v>7</v>
+      </c>
+      <c r="R220" t="n">
+        <v>0.1111111111111111</v>
+      </c>
+    </row>
+    <row r="221">
+      <c r="A221" t="inlineStr">
+        <is>
+          <t>2023-12-01 01:09:34</t>
+        </is>
+      </c>
+      <c r="B221" t="n">
+        <v>27</v>
+      </c>
+      <c r="C221" t="n">
+        <v>4</v>
+      </c>
+      <c r="D221" t="n">
+        <v>7</v>
+      </c>
+      <c r="E221" t="n">
+        <v>1</v>
+      </c>
+      <c r="F221" t="n">
+        <v>2</v>
+      </c>
+      <c r="G221" t="n">
+        <v>1</v>
+      </c>
+      <c r="H221" t="n">
+        <v>14</v>
+      </c>
+      <c r="I221" t="n">
+        <v>18</v>
+      </c>
+      <c r="J221" t="n">
+        <v>19</v>
+      </c>
+      <c r="K221" t="n">
+        <v>0.001</v>
+      </c>
+      <c r="L221" t="n">
+        <v>0.01</v>
+      </c>
+      <c r="M221" t="n">
+        <v>0.003</v>
+      </c>
+      <c r="N221" t="n">
+        <v>100</v>
+      </c>
+      <c r="O221" t="n">
+        <v>512</v>
+      </c>
+      <c r="P221" t="n">
+        <v>10</v>
+      </c>
+      <c r="Q221" t="n">
+        <v>7</v>
+      </c>
+      <c r="R221" t="n">
+        <v>0.1481481481481481</v>
+      </c>
+    </row>
+    <row r="222">
+      <c r="A222" t="inlineStr">
+        <is>
+          <t>2023-12-02 01:12:45</t>
+        </is>
+      </c>
+      <c r="B222" t="n">
+        <v>28</v>
+      </c>
+      <c r="C222" t="n">
+        <v>5</v>
+      </c>
+      <c r="D222" t="n">
+        <v>8</v>
+      </c>
+      <c r="E222" t="n">
+        <v>1</v>
+      </c>
+      <c r="F222" t="n">
+        <v>3</v>
+      </c>
+      <c r="G222" t="n">
+        <v>1</v>
+      </c>
+      <c r="H222" t="n">
+        <v>18</v>
+      </c>
+      <c r="I222" t="n">
+        <v>8</v>
+      </c>
+      <c r="J222" t="n">
+        <v>27</v>
+      </c>
+      <c r="K222" t="n">
+        <v>0.001</v>
+      </c>
+      <c r="L222" t="n">
+        <v>0.01</v>
+      </c>
+      <c r="M222" t="n">
+        <v>0.003</v>
+      </c>
+      <c r="N222" t="n">
+        <v>100</v>
+      </c>
+      <c r="O222" t="n">
+        <v>512</v>
+      </c>
+      <c r="P222" t="n">
+        <v>10</v>
+      </c>
+      <c r="Q222" t="n">
+        <v>7</v>
+      </c>
+      <c r="R222" t="n">
+        <v>0.1785714285714286</v>
+      </c>
+    </row>
+    <row r="223">
+      <c r="A223" t="inlineStr">
+        <is>
+          <t>2023-12-02 13:33:46</t>
+        </is>
+      </c>
+      <c r="B223" t="n">
+        <v>22</v>
+      </c>
+      <c r="C223" t="n">
+        <v>2</v>
+      </c>
+      <c r="D223" t="n">
+        <v>13</v>
+      </c>
+      <c r="E223" t="n">
+        <v>0</v>
+      </c>
+      <c r="F223" t="n">
+        <v>1</v>
+      </c>
+      <c r="G223" t="n">
+        <v>1</v>
+      </c>
+      <c r="H223" t="n">
+        <v>22</v>
+      </c>
+      <c r="I223" t="n">
+        <v>13</v>
+      </c>
+      <c r="J223" t="n">
+        <v>17</v>
+      </c>
+      <c r="K223" t="n">
+        <v>0.001</v>
+      </c>
+      <c r="L223" t="n">
+        <v>0.01</v>
+      </c>
+      <c r="M223" t="n">
+        <v>0.003</v>
+      </c>
+      <c r="N223" t="n">
+        <v>100</v>
+      </c>
+      <c r="O223" t="n">
+        <v>512</v>
+      </c>
+      <c r="P223" t="n">
+        <v>10</v>
+      </c>
+      <c r="Q223" t="n">
+        <v>7</v>
+      </c>
+      <c r="R223" t="n">
+        <v>0.09090909090909091</v>
+      </c>
+    </row>
+    <row r="224">
+      <c r="A224" t="inlineStr">
+        <is>
+          <t>2023-12-02 16:34:49</t>
+        </is>
+      </c>
+      <c r="B224" t="n">
+        <v>13</v>
+      </c>
+      <c r="C224" t="n">
+        <v>1</v>
+      </c>
+      <c r="D224" t="n">
+        <v>9</v>
+      </c>
+      <c r="E224" t="n">
+        <v>1</v>
+      </c>
+      <c r="F224" t="n">
+        <v>0</v>
+      </c>
+      <c r="G224" t="n">
+        <v>0</v>
+      </c>
+      <c r="H224" t="n">
+        <v>9</v>
+      </c>
+      <c r="I224" t="n">
+        <v>13</v>
+      </c>
+      <c r="J224" t="n">
+        <v>13</v>
+      </c>
+      <c r="K224" t="n">
+        <v>0.001</v>
+      </c>
+      <c r="L224" t="n">
+        <v>0.01</v>
+      </c>
+      <c r="M224" t="n">
+        <v>0.003</v>
+      </c>
+      <c r="N224" t="n">
+        <v>100</v>
+      </c>
+      <c r="O224" t="n">
+        <v>512</v>
+      </c>
+      <c r="P224" t="n">
+        <v>10</v>
+      </c>
+      <c r="Q224" t="n">
+        <v>7</v>
+      </c>
+      <c r="R224" t="n">
+        <v>0.07692307692307693</v>
+      </c>
+    </row>
+    <row r="225">
+      <c r="A225" t="inlineStr">
+        <is>
+          <t>2023-12-02 16:48:04</t>
+        </is>
+      </c>
+      <c r="B225" t="n">
+        <v>40</v>
+      </c>
+      <c r="C225" t="n">
+        <v>6</v>
+      </c>
+      <c r="D225" t="n">
+        <v>23</v>
+      </c>
+      <c r="E225" t="n">
+        <v>2</v>
+      </c>
+      <c r="F225" t="n">
+        <v>3</v>
+      </c>
+      <c r="G225" t="n">
+        <v>1</v>
+      </c>
+      <c r="H225" t="n">
+        <v>36</v>
+      </c>
+      <c r="I225" t="n">
+        <v>30</v>
+      </c>
+      <c r="J225" t="n">
+        <v>25</v>
+      </c>
+      <c r="K225" t="n">
+        <v>0.001</v>
+      </c>
+      <c r="L225" t="n">
+        <v>0.01</v>
+      </c>
+      <c r="M225" t="n">
+        <v>0.003</v>
+      </c>
+      <c r="N225" t="n">
+        <v>100</v>
+      </c>
+      <c r="O225" t="n">
+        <v>512</v>
+      </c>
+      <c r="P225" t="n">
+        <v>10</v>
+      </c>
+      <c r="Q225" t="n">
+        <v>7</v>
+      </c>
+      <c r="R225" t="n">
+        <v>0.15</v>
+      </c>
+    </row>
+    <row r="226">
+      <c r="A226" t="inlineStr">
+        <is>
+          <t>2023-12-02 20:27:47</t>
+        </is>
+      </c>
+      <c r="B226" t="n">
+        <v>98</v>
+      </c>
+      <c r="C226" t="n">
+        <v>15</v>
+      </c>
+      <c r="D226" t="n">
+        <v>22</v>
+      </c>
+      <c r="E226" t="n">
+        <v>4</v>
+      </c>
+      <c r="F226" t="n">
+        <v>4</v>
+      </c>
+      <c r="G226" t="n">
+        <v>7</v>
+      </c>
+      <c r="H226" t="n">
+        <v>35</v>
+      </c>
+      <c r="I226" t="n">
+        <v>62</v>
+      </c>
+      <c r="J226" t="n">
+        <v>24</v>
+      </c>
+      <c r="K226" t="n">
+        <v>0.001</v>
+      </c>
+      <c r="L226" t="n">
+        <v>0.01</v>
+      </c>
+      <c r="M226" t="n">
+        <v>0.003</v>
+      </c>
+      <c r="N226" t="n">
+        <v>100</v>
+      </c>
+      <c r="O226" t="n">
+        <v>512</v>
+      </c>
+      <c r="P226" t="n">
+        <v>10</v>
+      </c>
+      <c r="Q226" t="n">
+        <v>7</v>
+      </c>
+      <c r="R226" t="n">
+        <v>0.1530612244897959</v>
+      </c>
+    </row>
+    <row r="227">
+      <c r="A227" t="inlineStr">
+        <is>
+          <t>2023-12-03 15:12:19</t>
+        </is>
+      </c>
+      <c r="B227" t="n">
+        <v>2</v>
+      </c>
+      <c r="C227" t="n">
+        <v>0</v>
+      </c>
+      <c r="D227" t="n">
+        <v>2</v>
+      </c>
+      <c r="E227" t="n">
+        <v>0</v>
+      </c>
+      <c r="F227" t="n">
+        <v>0</v>
+      </c>
+      <c r="G227" t="n">
+        <v>0</v>
+      </c>
+      <c r="H227" t="n">
+        <v>2</v>
+      </c>
+      <c r="I227" t="n">
+        <v>2</v>
+      </c>
+      <c r="J227" t="n">
+        <v>2</v>
+      </c>
+      <c r="K227" t="n">
+        <v>0.001</v>
+      </c>
+      <c r="L227" t="n">
+        <v>0.01</v>
+      </c>
+      <c r="M227" t="n">
+        <v>0.003</v>
+      </c>
+      <c r="N227" t="n">
+        <v>100</v>
+      </c>
+      <c r="O227" t="n">
+        <v>512</v>
+      </c>
+      <c r="P227" t="n">
+        <v>10</v>
+      </c>
+      <c r="Q227" t="n">
+        <v>7</v>
+      </c>
+      <c r="R227" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="228">
+      <c r="A228" t="inlineStr">
+        <is>
+          <t>2023-12-05 00:00:45</t>
+        </is>
+      </c>
+      <c r="B228" t="n">
+        <v>18</v>
+      </c>
+      <c r="C228" t="n">
+        <v>3</v>
+      </c>
+      <c r="D228" t="n">
+        <v>6</v>
+      </c>
+      <c r="E228" t="n">
+        <v>0</v>
+      </c>
+      <c r="F228" t="n">
+        <v>2</v>
+      </c>
+      <c r="G228" t="n">
+        <v>1</v>
+      </c>
+      <c r="H228" t="n">
+        <v>18</v>
+      </c>
+      <c r="I228" t="n">
+        <v>8</v>
+      </c>
+      <c r="J228" t="n">
+        <v>16</v>
+      </c>
+      <c r="K228" t="n">
+        <v>0.001</v>
+      </c>
+      <c r="L228" t="n">
+        <v>0.01</v>
+      </c>
+      <c r="M228" t="n">
+        <v>0.003</v>
+      </c>
+      <c r="N228" t="n">
+        <v>100</v>
+      </c>
+      <c r="O228" t="n">
+        <v>512</v>
+      </c>
+      <c r="P228" t="n">
+        <v>10</v>
+      </c>
+      <c r="Q228" t="n">
+        <v>7</v>
+      </c>
+      <c r="R228" t="n">
+        <v>0.1666666666666667</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
sacar archivos programa y predictor y contador
</commit_message>
<xml_diff>
--- a/Reportes.xlsx
+++ b/Reportes.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:O3"/>
+  <dimension ref="A1:O6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -608,6 +608,153 @@
         <v>0.6666666666666666</v>
       </c>
     </row>
+    <row r="4">
+      <c r="A4" t="inlineStr">
+        <is>
+          <t>2023-12-10 19:20:33</t>
+        </is>
+      </c>
+      <c r="B4" t="n">
+        <v>13</v>
+      </c>
+      <c r="C4" t="n">
+        <v>12</v>
+      </c>
+      <c r="D4" t="n">
+        <v>4</v>
+      </c>
+      <c r="E4" t="n">
+        <v>3</v>
+      </c>
+      <c r="F4" t="n">
+        <v>5</v>
+      </c>
+      <c r="G4" t="n">
+        <v>0</v>
+      </c>
+      <c r="H4" t="n">
+        <v>0.001</v>
+      </c>
+      <c r="I4" t="n">
+        <v>0.01</v>
+      </c>
+      <c r="J4" t="n">
+        <v>0.003</v>
+      </c>
+      <c r="K4" t="n">
+        <v>100</v>
+      </c>
+      <c r="L4" t="n">
+        <v>512</v>
+      </c>
+      <c r="M4" t="n">
+        <v>10</v>
+      </c>
+      <c r="N4" t="n">
+        <v>7</v>
+      </c>
+      <c r="O4" t="n">
+        <v>0.9230769230769231</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="inlineStr">
+        <is>
+          <t>2023-12-10 21:05:03</t>
+        </is>
+      </c>
+      <c r="B5" t="n">
+        <v>11</v>
+      </c>
+      <c r="C5" t="n">
+        <v>6</v>
+      </c>
+      <c r="D5" t="n">
+        <v>1</v>
+      </c>
+      <c r="E5" t="n">
+        <v>0</v>
+      </c>
+      <c r="F5" t="n">
+        <v>5</v>
+      </c>
+      <c r="G5" t="n">
+        <v>0</v>
+      </c>
+      <c r="H5" t="n">
+        <v>0.001</v>
+      </c>
+      <c r="I5" t="n">
+        <v>0.01</v>
+      </c>
+      <c r="J5" t="n">
+        <v>0.003</v>
+      </c>
+      <c r="K5" t="n">
+        <v>100</v>
+      </c>
+      <c r="L5" t="n">
+        <v>512</v>
+      </c>
+      <c r="M5" t="n">
+        <v>10</v>
+      </c>
+      <c r="N5" t="n">
+        <v>7</v>
+      </c>
+      <c r="O5" t="n">
+        <v>0.5454545454545454</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="inlineStr">
+        <is>
+          <t>2023-12-10 22:30:25</t>
+        </is>
+      </c>
+      <c r="B6" t="n">
+        <v>25</v>
+      </c>
+      <c r="C6" t="n">
+        <v>19</v>
+      </c>
+      <c r="D6" t="n">
+        <v>6</v>
+      </c>
+      <c r="E6" t="n">
+        <v>2</v>
+      </c>
+      <c r="F6" t="n">
+        <v>11</v>
+      </c>
+      <c r="G6" t="n">
+        <v>0</v>
+      </c>
+      <c r="H6" t="n">
+        <v>0.001</v>
+      </c>
+      <c r="I6" t="n">
+        <v>0.01</v>
+      </c>
+      <c r="J6" t="n">
+        <v>0.003</v>
+      </c>
+      <c r="K6" t="n">
+        <v>100</v>
+      </c>
+      <c r="L6" t="n">
+        <v>512</v>
+      </c>
+      <c r="M6" t="n">
+        <v>10</v>
+      </c>
+      <c r="N6" t="n">
+        <v>7</v>
+      </c>
+      <c r="O6" t="n">
+        <v>0.76</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
se debe eliminar predictor
</commit_message>
<xml_diff>
--- a/Reportes.xlsx
+++ b/Reportes.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:O6"/>
+  <dimension ref="A1:O8"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -755,6 +755,104 @@
         <v>0.76</v>
       </c>
     </row>
+    <row r="7">
+      <c r="A7" t="inlineStr">
+        <is>
+          <t>2023-12-11 00:18:56</t>
+        </is>
+      </c>
+      <c r="B7" t="n">
+        <v>13</v>
+      </c>
+      <c r="C7" t="n">
+        <v>12</v>
+      </c>
+      <c r="D7" t="n">
+        <v>2</v>
+      </c>
+      <c r="E7" t="n">
+        <v>2</v>
+      </c>
+      <c r="F7" t="n">
+        <v>8</v>
+      </c>
+      <c r="G7" t="n">
+        <v>0</v>
+      </c>
+      <c r="H7" t="n">
+        <v>0.001</v>
+      </c>
+      <c r="I7" t="n">
+        <v>0.01</v>
+      </c>
+      <c r="J7" t="n">
+        <v>0.003</v>
+      </c>
+      <c r="K7" t="n">
+        <v>100</v>
+      </c>
+      <c r="L7" t="n">
+        <v>512</v>
+      </c>
+      <c r="M7" t="n">
+        <v>10</v>
+      </c>
+      <c r="N7" t="n">
+        <v>7</v>
+      </c>
+      <c r="O7" t="n">
+        <v>0.9230769230769231</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="inlineStr">
+        <is>
+          <t>2023-12-12 19:20:40</t>
+        </is>
+      </c>
+      <c r="B8" t="n">
+        <v>8</v>
+      </c>
+      <c r="C8" t="n">
+        <v>13</v>
+      </c>
+      <c r="D8" t="n">
+        <v>0</v>
+      </c>
+      <c r="E8" t="n">
+        <v>1</v>
+      </c>
+      <c r="F8" t="n">
+        <v>0</v>
+      </c>
+      <c r="G8" t="n">
+        <v>0</v>
+      </c>
+      <c r="H8" t="n">
+        <v>0.001</v>
+      </c>
+      <c r="I8" t="n">
+        <v>0.01</v>
+      </c>
+      <c r="J8" t="n">
+        <v>0.003</v>
+      </c>
+      <c r="K8" t="n">
+        <v>100</v>
+      </c>
+      <c r="L8" t="n">
+        <v>512</v>
+      </c>
+      <c r="M8" t="n">
+        <v>10</v>
+      </c>
+      <c r="N8" t="n">
+        <v>7</v>
+      </c>
+      <c r="O8" t="n">
+        <v>1.625</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
confiirmar los cambios falta mejorar el tema de borrado
</commit_message>
<xml_diff>
--- a/Reportes.xlsx
+++ b/Reportes.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:O8"/>
+  <dimension ref="A1:O11"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -853,6 +853,153 @@
         <v>1.625</v>
       </c>
     </row>
+    <row r="9">
+      <c r="A9" t="inlineStr">
+        <is>
+          <t>2023-12-15 01:16:26</t>
+        </is>
+      </c>
+      <c r="B9" t="n">
+        <v>7</v>
+      </c>
+      <c r="C9" t="n">
+        <v>6</v>
+      </c>
+      <c r="D9" t="n">
+        <v>3</v>
+      </c>
+      <c r="E9" t="n">
+        <v>2</v>
+      </c>
+      <c r="F9" t="n">
+        <v>0</v>
+      </c>
+      <c r="G9" t="n">
+        <v>1</v>
+      </c>
+      <c r="H9" t="n">
+        <v>0.001</v>
+      </c>
+      <c r="I9" t="n">
+        <v>0.01</v>
+      </c>
+      <c r="J9" t="n">
+        <v>0.003</v>
+      </c>
+      <c r="K9" t="n">
+        <v>100</v>
+      </c>
+      <c r="L9" t="n">
+        <v>512</v>
+      </c>
+      <c r="M9" t="n">
+        <v>10</v>
+      </c>
+      <c r="N9" t="n">
+        <v>7</v>
+      </c>
+      <c r="O9" t="n">
+        <v>0.8571428571428571</v>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" t="inlineStr">
+        <is>
+          <t>2023-12-15 01:21:13</t>
+        </is>
+      </c>
+      <c r="B10" t="n">
+        <v>3</v>
+      </c>
+      <c r="C10" t="n">
+        <v>3</v>
+      </c>
+      <c r="D10" t="n">
+        <v>1</v>
+      </c>
+      <c r="E10" t="n">
+        <v>1</v>
+      </c>
+      <c r="F10" t="n">
+        <v>0</v>
+      </c>
+      <c r="G10" t="n">
+        <v>0</v>
+      </c>
+      <c r="H10" t="n">
+        <v>0.001</v>
+      </c>
+      <c r="I10" t="n">
+        <v>0.01</v>
+      </c>
+      <c r="J10" t="n">
+        <v>0.003</v>
+      </c>
+      <c r="K10" t="n">
+        <v>100</v>
+      </c>
+      <c r="L10" t="n">
+        <v>512</v>
+      </c>
+      <c r="M10" t="n">
+        <v>10</v>
+      </c>
+      <c r="N10" t="n">
+        <v>7</v>
+      </c>
+      <c r="O10" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" t="inlineStr">
+        <is>
+          <t>2023-12-16 15:20:34</t>
+        </is>
+      </c>
+      <c r="B11" t="n">
+        <v>28</v>
+      </c>
+      <c r="C11" t="n">
+        <v>20</v>
+      </c>
+      <c r="D11" t="n">
+        <v>5</v>
+      </c>
+      <c r="E11" t="n">
+        <v>3</v>
+      </c>
+      <c r="F11" t="n">
+        <v>8</v>
+      </c>
+      <c r="G11" t="n">
+        <v>7</v>
+      </c>
+      <c r="H11" t="n">
+        <v>0.001</v>
+      </c>
+      <c r="I11" t="n">
+        <v>0.01</v>
+      </c>
+      <c r="J11" t="n">
+        <v>0.003</v>
+      </c>
+      <c r="K11" t="n">
+        <v>100</v>
+      </c>
+      <c r="L11" t="n">
+        <v>512</v>
+      </c>
+      <c r="M11" t="n">
+        <v>10</v>
+      </c>
+      <c r="N11" t="n">
+        <v>7</v>
+      </c>
+      <c r="O11" t="n">
+        <v>0.7142857142857143</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
guardar cambios y probar la ruleta
</commit_message>
<xml_diff>
--- a/Reportes.xlsx
+++ b/Reportes.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:O12"/>
+  <dimension ref="A1:O19"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1049,6 +1049,349 @@
         <v>0.6666666666666666</v>
       </c>
     </row>
+    <row r="13">
+      <c r="A13" t="inlineStr">
+        <is>
+          <t>2023-12-17 23:50:32</t>
+        </is>
+      </c>
+      <c r="B13" t="n">
+        <v>34</v>
+      </c>
+      <c r="C13" t="n">
+        <v>31</v>
+      </c>
+      <c r="D13" t="n">
+        <v>6</v>
+      </c>
+      <c r="E13" t="n">
+        <v>7</v>
+      </c>
+      <c r="F13" t="n">
+        <v>6</v>
+      </c>
+      <c r="G13" t="n">
+        <v>8</v>
+      </c>
+      <c r="H13" t="n">
+        <v>0.001</v>
+      </c>
+      <c r="I13" t="n">
+        <v>0.01</v>
+      </c>
+      <c r="J13" t="n">
+        <v>0.003</v>
+      </c>
+      <c r="K13" t="n">
+        <v>100</v>
+      </c>
+      <c r="L13" t="n">
+        <v>512</v>
+      </c>
+      <c r="M13" t="n">
+        <v>10</v>
+      </c>
+      <c r="N13" t="n">
+        <v>7</v>
+      </c>
+      <c r="O13" t="n">
+        <v>0.9117647058823529</v>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" t="inlineStr">
+        <is>
+          <t>2023-12-18 18:37:39</t>
+        </is>
+      </c>
+      <c r="B14" t="n">
+        <v>6</v>
+      </c>
+      <c r="C14" t="n">
+        <v>5</v>
+      </c>
+      <c r="D14" t="n">
+        <v>2</v>
+      </c>
+      <c r="E14" t="n">
+        <v>0</v>
+      </c>
+      <c r="F14" t="n">
+        <v>1</v>
+      </c>
+      <c r="G14" t="n">
+        <v>0</v>
+      </c>
+      <c r="H14" t="n">
+        <v>0.001</v>
+      </c>
+      <c r="I14" t="n">
+        <v>0.01</v>
+      </c>
+      <c r="J14" t="n">
+        <v>0.003</v>
+      </c>
+      <c r="K14" t="n">
+        <v>100</v>
+      </c>
+      <c r="L14" t="n">
+        <v>512</v>
+      </c>
+      <c r="M14" t="n">
+        <v>10</v>
+      </c>
+      <c r="N14" t="n">
+        <v>7</v>
+      </c>
+      <c r="O14" t="n">
+        <v>0.8333333333333334</v>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" t="inlineStr">
+        <is>
+          <t>2023-12-18 18:56:47</t>
+        </is>
+      </c>
+      <c r="B15" t="n">
+        <v>2</v>
+      </c>
+      <c r="C15" t="n">
+        <v>2</v>
+      </c>
+      <c r="D15" t="n">
+        <v>1</v>
+      </c>
+      <c r="E15" t="n">
+        <v>0</v>
+      </c>
+      <c r="F15" t="n">
+        <v>0</v>
+      </c>
+      <c r="G15" t="n">
+        <v>1</v>
+      </c>
+      <c r="H15" t="n">
+        <v>0.001</v>
+      </c>
+      <c r="I15" t="n">
+        <v>0.01</v>
+      </c>
+      <c r="J15" t="n">
+        <v>0.003</v>
+      </c>
+      <c r="K15" t="n">
+        <v>100</v>
+      </c>
+      <c r="L15" t="n">
+        <v>512</v>
+      </c>
+      <c r="M15" t="n">
+        <v>10</v>
+      </c>
+      <c r="N15" t="n">
+        <v>7</v>
+      </c>
+      <c r="O15" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" t="inlineStr">
+        <is>
+          <t>2023-12-19 00:43:14</t>
+        </is>
+      </c>
+      <c r="B16" t="n">
+        <v>15</v>
+      </c>
+      <c r="C16" t="n">
+        <v>12</v>
+      </c>
+      <c r="D16" t="n">
+        <v>3</v>
+      </c>
+      <c r="E16" t="n">
+        <v>1</v>
+      </c>
+      <c r="F16" t="n">
+        <v>3</v>
+      </c>
+      <c r="G16" t="n">
+        <v>5</v>
+      </c>
+      <c r="H16" t="n">
+        <v>0.001</v>
+      </c>
+      <c r="I16" t="n">
+        <v>0.01</v>
+      </c>
+      <c r="J16" t="n">
+        <v>0.003</v>
+      </c>
+      <c r="K16" t="n">
+        <v>100</v>
+      </c>
+      <c r="L16" t="n">
+        <v>512</v>
+      </c>
+      <c r="M16" t="n">
+        <v>10</v>
+      </c>
+      <c r="N16" t="n">
+        <v>7</v>
+      </c>
+      <c r="O16" t="n">
+        <v>0.8</v>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17" t="inlineStr">
+        <is>
+          <t>2023-12-19 01:16:00</t>
+        </is>
+      </c>
+      <c r="B17" t="n">
+        <v>7</v>
+      </c>
+      <c r="C17" t="n">
+        <v>5</v>
+      </c>
+      <c r="D17" t="n">
+        <v>1</v>
+      </c>
+      <c r="E17" t="n">
+        <v>0</v>
+      </c>
+      <c r="F17" t="n">
+        <v>2</v>
+      </c>
+      <c r="G17" t="n">
+        <v>2</v>
+      </c>
+      <c r="H17" t="n">
+        <v>0.001</v>
+      </c>
+      <c r="I17" t="n">
+        <v>0.01</v>
+      </c>
+      <c r="J17" t="n">
+        <v>0.003</v>
+      </c>
+      <c r="K17" t="n">
+        <v>100</v>
+      </c>
+      <c r="L17" t="n">
+        <v>512</v>
+      </c>
+      <c r="M17" t="n">
+        <v>10</v>
+      </c>
+      <c r="N17" t="n">
+        <v>7</v>
+      </c>
+      <c r="O17" t="n">
+        <v>0.7142857142857143</v>
+      </c>
+    </row>
+    <row r="18">
+      <c r="A18" t="inlineStr">
+        <is>
+          <t>2023-12-21 07:21:25</t>
+        </is>
+      </c>
+      <c r="B18" t="n">
+        <v>11</v>
+      </c>
+      <c r="C18" t="n">
+        <v>7</v>
+      </c>
+      <c r="D18" t="n">
+        <v>1</v>
+      </c>
+      <c r="E18" t="n">
+        <v>0</v>
+      </c>
+      <c r="F18" t="n">
+        <v>2</v>
+      </c>
+      <c r="G18" t="n">
+        <v>2</v>
+      </c>
+      <c r="H18" t="n">
+        <v>0.001</v>
+      </c>
+      <c r="I18" t="n">
+        <v>0.01</v>
+      </c>
+      <c r="J18" t="n">
+        <v>0.003</v>
+      </c>
+      <c r="K18" t="n">
+        <v>100</v>
+      </c>
+      <c r="L18" t="n">
+        <v>512</v>
+      </c>
+      <c r="M18" t="n">
+        <v>10</v>
+      </c>
+      <c r="N18" t="n">
+        <v>7</v>
+      </c>
+      <c r="O18" t="n">
+        <v>0.6363636363636364</v>
+      </c>
+    </row>
+    <row r="19">
+      <c r="A19" t="inlineStr">
+        <is>
+          <t>2023-12-22 22:48:45</t>
+        </is>
+      </c>
+      <c r="B19" t="n">
+        <v>11</v>
+      </c>
+      <c r="C19" t="n">
+        <v>8</v>
+      </c>
+      <c r="D19" t="n">
+        <v>2</v>
+      </c>
+      <c r="E19" t="n">
+        <v>3</v>
+      </c>
+      <c r="F19" t="n">
+        <v>2</v>
+      </c>
+      <c r="G19" t="n">
+        <v>1</v>
+      </c>
+      <c r="H19" t="n">
+        <v>0.001</v>
+      </c>
+      <c r="I19" t="n">
+        <v>0.01</v>
+      </c>
+      <c r="J19" t="n">
+        <v>0.003</v>
+      </c>
+      <c r="K19" t="n">
+        <v>100</v>
+      </c>
+      <c r="L19" t="n">
+        <v>512</v>
+      </c>
+      <c r="M19" t="n">
+        <v>10</v>
+      </c>
+      <c r="N19" t="n">
+        <v>7</v>
+      </c>
+      <c r="O19" t="n">
+        <v>0.7272727272727273</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
falta agregar una vez que se encuentra en resultados ir sumando las probabilidades si es que ya  en resultados
</commit_message>
<xml_diff>
--- a/Reportes.xlsx
+++ b/Reportes.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:Q93"/>
+  <dimension ref="A1:Q95"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -5654,6 +5654,116 @@
         </is>
       </c>
     </row>
+    <row r="94">
+      <c r="A94" t="inlineStr">
+        <is>
+          <t>2024-01-15 18:58:58</t>
+        </is>
+      </c>
+      <c r="B94" t="n">
+        <v>13</v>
+      </c>
+      <c r="C94" t="n">
+        <v>13</v>
+      </c>
+      <c r="D94" t="n">
+        <v>2</v>
+      </c>
+      <c r="E94" t="n">
+        <v>3</v>
+      </c>
+      <c r="F94" t="n">
+        <v>6</v>
+      </c>
+      <c r="G94" t="n">
+        <v>2</v>
+      </c>
+      <c r="H94" t="n">
+        <v>0</v>
+      </c>
+      <c r="I94" t="n">
+        <v>0.001</v>
+      </c>
+      <c r="J94" t="n">
+        <v>0.05</v>
+      </c>
+      <c r="K94" t="n">
+        <v>0.003</v>
+      </c>
+      <c r="L94" t="n">
+        <v>100</v>
+      </c>
+      <c r="M94" t="n">
+        <v>500</v>
+      </c>
+      <c r="N94" t="n">
+        <v>10</v>
+      </c>
+      <c r="O94" t="n">
+        <v>5</v>
+      </c>
+      <c r="P94" t="inlineStr"/>
+      <c r="Q94" t="inlineStr">
+        <is>
+          <t>Data/bombay2.xlsx</t>
+        </is>
+      </c>
+    </row>
+    <row r="95">
+      <c r="A95" t="inlineStr">
+        <is>
+          <t>2024-01-16 13:32:44</t>
+        </is>
+      </c>
+      <c r="B95" t="n">
+        <v>69</v>
+      </c>
+      <c r="C95" t="n">
+        <v>52</v>
+      </c>
+      <c r="D95" t="n">
+        <v>8</v>
+      </c>
+      <c r="E95" t="n">
+        <v>20</v>
+      </c>
+      <c r="F95" t="n">
+        <v>15</v>
+      </c>
+      <c r="G95" t="n">
+        <v>9</v>
+      </c>
+      <c r="H95" t="n">
+        <v>0</v>
+      </c>
+      <c r="I95" t="n">
+        <v>0.001</v>
+      </c>
+      <c r="J95" t="n">
+        <v>0.05</v>
+      </c>
+      <c r="K95" t="n">
+        <v>0.003</v>
+      </c>
+      <c r="L95" t="n">
+        <v>100</v>
+      </c>
+      <c r="M95" t="n">
+        <v>500</v>
+      </c>
+      <c r="N95" t="n">
+        <v>10</v>
+      </c>
+      <c r="O95" t="n">
+        <v>5</v>
+      </c>
+      <c r="P95" t="inlineStr"/>
+      <c r="Q95" t="inlineStr">
+        <is>
+          <t>Data/bombay1.xlsx</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>